<commit_message>
Test support + gitignore edit
</commit_message>
<xml_diff>
--- a/Quoting/templates/Product_Configs_Provar.xlsx
+++ b/Quoting/templates/Product_Configs_Provar.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="23520" windowHeight="10650"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="23520" windowHeight="10650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ProductConfigs" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1846" uniqueCount="315">
   <si>
     <t>Agency</t>
   </si>
@@ -2770,8 +2770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EW1492"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="EI1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="EV3" sqref="EV3"/>
+    <sheetView showGridLines="0" topLeftCell="A102" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -3451,7 +3451,7 @@
       <c r="N3" s="26"/>
       <c r="O3" s="28">
         <f ca="1">TODAY()</f>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P3" s="26"/>
       <c r="Q3" s="26"/>
@@ -3713,7 +3713,7 @@
       <c r="N5" s="26"/>
       <c r="O5" s="28">
         <f ca="1">TODAY()</f>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P5" s="26"/>
       <c r="Q5" s="26"/>
@@ -3909,7 +3909,7 @@
       <c r="N6" s="26"/>
       <c r="O6" s="28">
         <f t="shared" ref="O6:O96" ca="1" si="0">TODAY()</f>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P6" s="26"/>
       <c r="Q6" s="26"/>
@@ -4119,7 +4119,7 @@
       <c r="N7" s="26"/>
       <c r="O7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P7" s="26"/>
       <c r="Q7" s="26"/>
@@ -4346,7 +4346,7 @@
       <c r="N8" s="45"/>
       <c r="O8" s="47">
         <f t="shared" ref="O8:O77" ca="1" si="1">TODAY()</f>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P8" s="45"/>
       <c r="Q8" s="45"/>
@@ -4552,7 +4552,7 @@
       <c r="N9" s="26"/>
       <c r="O9" s="28">
         <f t="shared" ref="O9:O118" ca="1" si="2">TODAY()</f>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P9" s="26"/>
       <c r="Q9" s="26"/>
@@ -4718,7 +4718,7 @@
       <c r="N10" s="26"/>
       <c r="O10" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P10" s="26"/>
       <c r="Q10" s="26"/>
@@ -4884,7 +4884,7 @@
       <c r="N11" s="26"/>
       <c r="O11" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P11" s="26"/>
       <c r="Q11" s="26"/>
@@ -5052,7 +5052,7 @@
       <c r="N12" s="26"/>
       <c r="O12" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P12" s="26"/>
       <c r="Q12" s="26"/>
@@ -5234,7 +5234,7 @@
       <c r="N13" s="26"/>
       <c r="O13" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P13" s="26"/>
       <c r="Q13" s="26"/>
@@ -5466,7 +5466,7 @@
       <c r="N14" s="26"/>
       <c r="O14" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P14" s="26"/>
       <c r="Q14" s="26"/>
@@ -5697,7 +5697,7 @@
       <c r="N15" s="45"/>
       <c r="O15" s="47">
         <f t="shared" ref="O15:O55" ca="1" si="3">TODAY()</f>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P15" s="45"/>
       <c r="Q15" s="45"/>
@@ -5903,7 +5903,7 @@
       <c r="N16" s="26"/>
       <c r="O16" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P16" s="26"/>
       <c r="Q16" s="26"/>
@@ -6073,7 +6073,7 @@
       <c r="N17" s="26"/>
       <c r="O17" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P17" s="26"/>
       <c r="Q17" s="26"/>
@@ -6301,7 +6301,7 @@
       <c r="N18" s="26"/>
       <c r="O18" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P18" s="26"/>
       <c r="Q18" s="26"/>
@@ -6528,7 +6528,7 @@
       <c r="N19" s="45"/>
       <c r="O19" s="47">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P19" s="45"/>
       <c r="Q19" s="45"/>
@@ -6708,7 +6708,7 @@
       <c r="N20" s="26"/>
       <c r="O20" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P20" s="26"/>
       <c r="Q20" s="26"/>
@@ -6876,7 +6876,7 @@
       <c r="N21" s="26"/>
       <c r="O21" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P21" s="26"/>
       <c r="Q21" s="26"/>
@@ -7056,7 +7056,7 @@
       <c r="N22" s="26"/>
       <c r="O22" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P22" s="26"/>
       <c r="Q22" s="26"/>
@@ -7280,7 +7280,7 @@
       <c r="N23" s="26"/>
       <c r="O23" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P23" s="26"/>
       <c r="Q23" s="26"/>
@@ -7460,7 +7460,7 @@
       <c r="N24" s="26"/>
       <c r="O24" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P24" s="26"/>
       <c r="Q24" s="26"/>
@@ -7650,7 +7650,7 @@
       <c r="N25" s="26"/>
       <c r="O25" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P25" s="26" t="s">
         <v>240</v>
@@ -7836,7 +7836,7 @@
       <c r="N26" s="26"/>
       <c r="O26" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P26" s="26"/>
       <c r="Q26" s="26"/>
@@ -8012,7 +8012,7 @@
       <c r="N27" s="26"/>
       <c r="O27" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P27" s="26"/>
       <c r="Q27" s="26"/>
@@ -8186,7 +8186,7 @@
       <c r="N28" s="26"/>
       <c r="O28" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P28" s="26"/>
       <c r="Q28" s="26"/>
@@ -8374,7 +8374,7 @@
       <c r="N29" s="26"/>
       <c r="O29" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P29" s="26"/>
       <c r="Q29" s="26"/>
@@ -8548,7 +8548,7 @@
       <c r="N30" s="26"/>
       <c r="O30" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P30" s="26"/>
       <c r="Q30" s="26"/>
@@ -8758,7 +8758,7 @@
       </c>
       <c r="O31" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="S31" s="43" t="s">
         <v>6</v>
@@ -8848,7 +8848,7 @@
       </c>
       <c r="O32" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="R32" s="42" t="s">
         <v>6</v>
@@ -9004,7 +9004,7 @@
       <c r="N33" s="26"/>
       <c r="O33" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P33" s="26"/>
       <c r="Q33" s="26"/>
@@ -9170,7 +9170,7 @@
       <c r="N34" s="26"/>
       <c r="O34" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P34" s="26"/>
       <c r="Q34" s="26"/>
@@ -9336,7 +9336,7 @@
       <c r="N35" s="26"/>
       <c r="O35" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P35" s="26"/>
       <c r="Q35" s="26"/>
@@ -9502,7 +9502,7 @@
       <c r="N36" s="26"/>
       <c r="O36" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P36" s="26"/>
       <c r="Q36" s="26"/>
@@ -9674,7 +9674,7 @@
       <c r="N37" s="26"/>
       <c r="O37" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P37" s="26"/>
       <c r="Q37" s="26"/>
@@ -9850,7 +9850,7 @@
       <c r="N38" s="26"/>
       <c r="O38" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P38" s="26"/>
       <c r="Q38" s="26"/>
@@ -10025,7 +10025,7 @@
       <c r="N39" s="45"/>
       <c r="O39" s="47">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P39" s="45"/>
       <c r="Q39" s="45"/>
@@ -10238,7 +10238,7 @@
       <c r="N40" s="45"/>
       <c r="O40" s="47">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P40" s="45"/>
       <c r="Q40" s="45"/>
@@ -10448,7 +10448,7 @@
       <c r="N41" s="26"/>
       <c r="O41" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P41" s="26"/>
       <c r="Q41" s="26"/>
@@ -10647,7 +10647,7 @@
       <c r="N42" s="45"/>
       <c r="O42" s="47">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P42" s="45"/>
       <c r="Q42" s="45"/>
@@ -10849,7 +10849,7 @@
       <c r="N43" s="26"/>
       <c r="O43" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P43" s="26"/>
       <c r="Q43" s="26"/>
@@ -11019,7 +11019,7 @@
       <c r="N44" s="26"/>
       <c r="O44" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P44" s="26"/>
       <c r="Q44" s="26"/>
@@ -11185,7 +11185,7 @@
       <c r="N45" s="26"/>
       <c r="O45" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P45" s="26"/>
       <c r="Q45" s="26"/>
@@ -11350,7 +11350,7 @@
       <c r="N46" s="45"/>
       <c r="O46" s="47">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P46" s="45"/>
       <c r="Q46" s="45"/>
@@ -11517,7 +11517,7 @@
       <c r="N47" s="45"/>
       <c r="O47" s="47">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P47" s="45"/>
       <c r="Q47" s="45"/>
@@ -11682,7 +11682,7 @@
       <c r="N48" s="1"/>
       <c r="O48" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
@@ -11885,7 +11885,7 @@
       <c r="N49" s="1"/>
       <c r="O49" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
@@ -12121,7 +12121,7 @@
       <c r="N50" s="33"/>
       <c r="O50" s="52">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P50" s="33"/>
       <c r="Q50" s="33"/>
@@ -12354,7 +12354,7 @@
       <c r="N51" s="1"/>
       <c r="O51" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
@@ -12571,7 +12571,7 @@
       <c r="N52" s="1"/>
       <c r="O52" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
@@ -12782,7 +12782,7 @@
       <c r="N53" s="1"/>
       <c r="O53" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
@@ -12993,7 +12993,7 @@
       <c r="N54" s="1"/>
       <c r="O54" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
@@ -13176,7 +13176,7 @@
       <c r="N55" s="1"/>
       <c r="O55" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P55" s="1"/>
       <c r="Q55" s="1"/>
@@ -13361,7 +13361,7 @@
       <c r="N56" s="1"/>
       <c r="O56" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
@@ -13582,7 +13582,7 @@
       <c r="N57" s="1"/>
       <c r="O57" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
@@ -13815,7 +13815,7 @@
       <c r="N58" s="1"/>
       <c r="O58" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
@@ -14032,7 +14032,7 @@
       <c r="N59" s="1"/>
       <c r="O59" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
@@ -14221,7 +14221,7 @@
       <c r="N60" s="1"/>
       <c r="O60" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
@@ -14404,7 +14404,7 @@
       <c r="N61" s="1"/>
       <c r="O61" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
@@ -14601,7 +14601,7 @@
       <c r="N62" s="1"/>
       <c r="O62" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
@@ -14832,7 +14832,7 @@
       <c r="N63" s="1"/>
       <c r="O63" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P63" s="1"/>
       <c r="Q63" s="1"/>
@@ -15063,7 +15063,7 @@
       <c r="N64" s="1"/>
       <c r="O64" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
@@ -15250,7 +15250,7 @@
       <c r="N65" s="1"/>
       <c r="O65" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P65" s="1"/>
       <c r="Q65" s="1"/>
@@ -15439,7 +15439,7 @@
       <c r="N66" s="1"/>
       <c r="O66" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
@@ -15626,7 +15626,7 @@
       <c r="N67" s="1"/>
       <c r="O67" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
@@ -15807,7 +15807,7 @@
       <c r="N68" s="1"/>
       <c r="O68" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
@@ -15974,7 +15974,7 @@
       <c r="N69" s="1"/>
       <c r="O69" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P69" s="1"/>
       <c r="Q69" s="1"/>
@@ -16142,7 +16142,7 @@
       <c r="N70" s="26"/>
       <c r="O70" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P70" s="26"/>
       <c r="Q70" s="26"/>
@@ -16314,7 +16314,7 @@
       <c r="N71" s="1"/>
       <c r="O71" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P71" s="1"/>
       <c r="Q71" s="1"/>
@@ -16523,7 +16523,7 @@
       <c r="N72" s="1"/>
       <c r="O72" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
@@ -16696,7 +16696,7 @@
       <c r="N73" s="1"/>
       <c r="O73" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P73" s="1"/>
       <c r="Q73" s="1"/>
@@ -16871,7 +16871,7 @@
       <c r="N74" s="1"/>
       <c r="O74" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
@@ -17082,7 +17082,7 @@
       <c r="N75" s="1"/>
       <c r="O75" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P75" s="1"/>
       <c r="Q75" s="1"/>
@@ -17291,7 +17291,7 @@
       <c r="N76" s="1"/>
       <c r="O76" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P76" s="1"/>
       <c r="Q76" s="1"/>
@@ -17498,7 +17498,7 @@
       <c r="N77" s="1"/>
       <c r="O77" s="28">
         <f t="shared" ca="1" si="1"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P77" s="1"/>
       <c r="Q77" s="1"/>
@@ -17730,7 +17730,7 @@
       <c r="N78" s="1"/>
       <c r="O78" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P78" s="1"/>
       <c r="Q78" s="1"/>
@@ -17944,7 +17944,7 @@
       <c r="N79" s="1"/>
       <c r="O79" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P79" s="1"/>
       <c r="Q79" s="1"/>
@@ -18160,7 +18160,7 @@
       <c r="N80" s="1"/>
       <c r="O80" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P80" s="1"/>
       <c r="Q80" s="1"/>
@@ -18378,7 +18378,7 @@
       <c r="N81" s="45"/>
       <c r="O81" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P81" s="45"/>
       <c r="Q81" s="45"/>
@@ -18585,7 +18585,7 @@
       <c r="N82" s="1"/>
       <c r="O82" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P82" s="1"/>
       <c r="Q82" s="1"/>
@@ -18750,7 +18750,7 @@
       <c r="N83" s="1"/>
       <c r="O83" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
@@ -18915,7 +18915,7 @@
       <c r="N84" s="1"/>
       <c r="O84" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P84" s="1"/>
       <c r="Q84" s="1"/>
@@ -19084,7 +19084,7 @@
       <c r="N85" s="1"/>
       <c r="O85" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P85" s="1"/>
       <c r="Q85" s="1"/>
@@ -19311,7 +19311,7 @@
       <c r="N86" s="1"/>
       <c r="O86" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P86" s="1"/>
       <c r="Q86" s="1"/>
@@ -19538,7 +19538,7 @@
       <c r="N87" s="1"/>
       <c r="O87" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P87" s="1"/>
       <c r="Q87" s="1"/>
@@ -19749,7 +19749,7 @@
       <c r="N88" s="45"/>
       <c r="O88" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P88" s="45"/>
       <c r="Q88" s="45"/>
@@ -19956,7 +19956,7 @@
       <c r="N89" s="1"/>
       <c r="O89" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P89" s="1"/>
       <c r="Q89" s="1"/>
@@ -20163,7 +20163,7 @@
       <c r="N90" s="1"/>
       <c r="O90" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P90" s="1"/>
       <c r="Q90" s="1"/>
@@ -20360,7 +20360,7 @@
       <c r="N91" s="1"/>
       <c r="O91" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P91" s="1"/>
       <c r="Q91" s="1"/>
@@ -20587,7 +20587,7 @@
       <c r="N92" s="1"/>
       <c r="O92" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P92" s="1"/>
       <c r="Q92" s="1"/>
@@ -20814,7 +20814,7 @@
       <c r="N93" s="1"/>
       <c r="O93" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P93" s="1"/>
       <c r="Q93" s="1"/>
@@ -21037,7 +21037,7 @@
       <c r="N94" s="1"/>
       <c r="O94" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P94" s="1"/>
       <c r="Q94" s="1"/>
@@ -21204,7 +21204,7 @@
       <c r="N95" s="1"/>
       <c r="O95" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P95" s="1"/>
       <c r="Q95" s="1"/>
@@ -21371,7 +21371,7 @@
       <c r="N96" s="1"/>
       <c r="O96" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P96" s="1"/>
       <c r="Q96" s="1"/>
@@ -21696,7 +21696,7 @@
       <c r="N98" s="1"/>
       <c r="O98" s="28">
         <f ca="1">TODAY()</f>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P98" s="1"/>
       <c r="Q98" s="1"/>
@@ -22023,7 +22023,7 @@
       <c r="N100" s="1"/>
       <c r="O100" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P100" s="1"/>
       <c r="Q100" s="1"/>
@@ -22214,7 +22214,7 @@
       <c r="N101" s="1"/>
       <c r="O101" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P101" s="1"/>
       <c r="Q101" s="1"/>
@@ -22407,7 +22407,7 @@
       <c r="N102" s="1"/>
       <c r="O102" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P102" s="1"/>
       <c r="Q102" s="1"/>
@@ -22592,7 +22592,7 @@
       <c r="N103" s="1"/>
       <c r="O103" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P103" s="1"/>
       <c r="Q103" s="1"/>
@@ -22767,7 +22767,7 @@
       <c r="N104" s="1"/>
       <c r="O104" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P104" s="1"/>
       <c r="Q104" s="1"/>
@@ -22944,7 +22944,7 @@
       <c r="N105" s="1"/>
       <c r="O105" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P105" s="1"/>
       <c r="Q105" s="1"/>
@@ -23121,7 +23121,7 @@
       <c r="N106" s="1"/>
       <c r="O106" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P106" s="1"/>
       <c r="Q106" s="1"/>
@@ -23298,7 +23298,7 @@
       <c r="N107" s="1"/>
       <c r="O107" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P107" s="1"/>
       <c r="Q107" s="1"/>
@@ -23475,7 +23475,7 @@
       <c r="N108" s="1"/>
       <c r="O108" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P108" s="1"/>
       <c r="Q108" s="1"/>
@@ -23652,7 +23652,7 @@
       <c r="N109" s="1"/>
       <c r="O109" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P109" s="1"/>
       <c r="Q109" s="1"/>
@@ -23845,7 +23845,7 @@
       <c r="N110" s="1"/>
       <c r="O110" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P110" s="1"/>
       <c r="Q110" s="1"/>
@@ -24038,7 +24038,7 @@
       <c r="N111" s="1"/>
       <c r="O111" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P111" s="1"/>
       <c r="Q111" s="1"/>
@@ -24231,7 +24231,7 @@
       <c r="N112" s="1"/>
       <c r="O112" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P112" s="1"/>
       <c r="Q112" s="1"/>
@@ -24424,7 +24424,7 @@
       <c r="N113" s="1"/>
       <c r="O113" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P113" s="1"/>
       <c r="Q113" s="1"/>
@@ -24617,7 +24617,7 @@
       <c r="N114" s="1"/>
       <c r="O114" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P114" s="1"/>
       <c r="Q114" s="1"/>
@@ -24810,7 +24810,7 @@
       <c r="N115" s="1"/>
       <c r="O115" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P115" s="1"/>
       <c r="Q115" s="1"/>
@@ -25003,7 +25003,7 @@
       <c r="N116" s="1"/>
       <c r="O116" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P116" s="1"/>
       <c r="Q116" s="1"/>
@@ -25196,7 +25196,7 @@
       <c r="N117" s="1"/>
       <c r="O117" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P117" s="1"/>
       <c r="Q117" s="1"/>
@@ -25389,7 +25389,7 @@
       <c r="N118" s="1"/>
       <c r="O118" s="28">
         <f t="shared" ca="1" si="2"/>
-        <v>42466</v>
+        <v>42472</v>
       </c>
       <c r="P118" s="1"/>
       <c r="Q118" s="1"/>
@@ -53017,8 +53017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53088,6 +53088,9 @@
       <c r="D2" s="43" t="s">
         <v>35</v>
       </c>
+      <c r="E2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>

</xml_diff>